<commit_message>
bug fix: senior editor schedule generator no longer asks for dispay name
</commit_message>
<xml_diff>
--- a/schedule_with_senior_editors.xlsx
+++ b/schedule_with_senior_editors.xlsx
@@ -471,12 +471,12 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>test1</t>
+          <t>Daisy</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>Tak</t>
         </is>
       </c>
     </row>
@@ -488,7 +488,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -498,7 +498,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -518,12 +518,12 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -565,12 +565,12 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -602,22 +602,22 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>off</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -634,12 +634,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -659,12 +659,12 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -706,12 +706,12 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -723,7 +723,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -753,12 +753,12 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -780,32 +780,32 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -822,12 +822,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -847,12 +847,12 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -889,17 +889,17 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -936,17 +936,17 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -973,27 +973,27 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -1035,12 +1035,12 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -1082,12 +1082,12 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -1119,7 +1119,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1129,12 +1129,12 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -1171,17 +1171,17 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -1223,12 +1223,12 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1270,12 +1270,12 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -1297,17 +1297,17 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1317,12 +1317,12 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -1339,22 +1339,22 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1364,12 +1364,12 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -1381,7 +1381,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1396,12 +1396,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1411,12 +1411,12 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -1458,12 +1458,12 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -1505,12 +1505,12 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -1552,12 +1552,12 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -1599,12 +1599,12 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -1646,12 +1646,12 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -1678,7 +1678,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1688,17 +1688,17 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>off</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -1710,7 +1710,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1735,17 +1735,17 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -1787,12 +1787,12 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -1834,12 +1834,12 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -1881,12 +1881,12 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Freelancer weekday dayshift changed to 0930-1830
</commit_message>
<xml_diff>
--- a/schedule_with_senior_editors.xlsx
+++ b/schedule_with_senior_editors.xlsx
@@ -513,7 +513,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -535,7 +535,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -607,7 +607,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -639,7 +639,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -691,7 +691,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -822,7 +822,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -869,7 +869,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -936,7 +936,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -978,7 +978,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1030,7 +1030,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1146,7 +1146,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1218,17 +1218,17 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>13-22</t>
         </is>
       </c>
     </row>
@@ -1265,7 +1265,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1339,7 +1339,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1485,7 +1485,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1522,7 +1522,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1579,7 +1579,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1626,7 +1626,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1814,7 +1814,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1861,7 +1861,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">

</xml_diff>

<commit_message>
generate_fulltime_schedule replaced the old senior editor scheduler
</commit_message>
<xml_diff>
--- a/schedule_with_senior_editors.xlsx
+++ b/schedule_with_senior_editors.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,41 @@
           <t>Tak</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Waiyee</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Cindy</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Ivy</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Aasta</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Carol</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Jackie</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Tiffany</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -488,24 +523,24 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>7-16</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>off</t>
@@ -513,17 +548,52 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0930-1830</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>CL</t>
         </is>
       </c>
     </row>
@@ -535,42 +605,77 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>0930-1830</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>off</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -582,42 +687,77 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0930-1830</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>7-16</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>0930-1830</t>
-        </is>
-      </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -629,42 +769,77 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>7-16</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>0930-1830</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
       <c r="H5" t="inlineStr">
         <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
           <t>13-22</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>13-22</t>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>PH</t>
         </is>
       </c>
     </row>
@@ -676,27 +851,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>off</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0930-1830</t>
+          <t>off</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -706,12 +881,47 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
           <t>13-22</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>13-22</t>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -723,7 +933,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -733,32 +943,67 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
           <t>7-16</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>10-19</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>自由調配</t>
         </is>
       </c>
     </row>
@@ -775,24 +1020,24 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
           <t>7-16</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>10-19</t>
-        </is>
-      </c>
       <c r="G8" t="inlineStr">
         <is>
           <t>off</t>
@@ -800,12 +1045,47 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>PH</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -817,42 +1097,77 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>0930-1830</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>7-16</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
       <c r="H9" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
           <t>13-22</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>13-22</t>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -864,42 +1179,77 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
           <t>0930-1830</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
           <t>13-22</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>13-22</t>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>AL</t>
         </is>
       </c>
     </row>
@@ -916,37 +1266,72 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>0930-1830</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>7-16</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>0930-1830</t>
-        </is>
-      </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>CL</t>
         </is>
       </c>
     </row>
@@ -958,12 +1343,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -978,22 +1363,57 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>0930-1830</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>off</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1005,27 +1425,27 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>off</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1035,12 +1455,47 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>AL</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1052,12 +1507,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1077,17 +1532,52 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
           <t>13-22</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>13-22</t>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>PH</t>
         </is>
       </c>
     </row>
@@ -1099,17 +1589,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1119,22 +1609,57 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>7-16</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
       <c r="H15" t="inlineStr">
         <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
           <t>13-22</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>13-22</t>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1146,42 +1671,77 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>0930-1830</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>off</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>自由調配</t>
         </is>
       </c>
     </row>
@@ -1193,22 +1753,22 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>7-16</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1223,12 +1783,47 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>PH</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1240,42 +1835,77 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
           <t>7-16</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>0930-1830</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
           <t>13-22</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>13-22</t>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1297,14 +1927,14 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
           <t>0930-1830</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
       <c r="F19" t="inlineStr">
         <is>
           <t>15-24</t>
@@ -1312,17 +1942,52 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
           <t>13-22</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>13-22</t>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>AL</t>
         </is>
       </c>
     </row>
@@ -1334,42 +1999,77 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
+          <t>0930-1830</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
           <t>7-16</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>0930-1830</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>CL</t>
         </is>
       </c>
     </row>
@@ -1381,19 +2081,19 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
           <t>7-16</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
       <c r="E21" t="inlineStr">
         <is>
           <t>10-19</t>
@@ -1411,12 +2111,47 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1433,7 +2168,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1453,17 +2188,52 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>AL</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1480,37 +2250,72 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
           <t>0930-1830</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
         <is>
           <t>7-16</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
       <c r="H23" t="inlineStr">
         <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
           <t>13-22</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>13-22</t>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>PH</t>
         </is>
       </c>
     </row>
@@ -1522,27 +2327,27 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>7-16</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
           <t>0930-1830</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1552,12 +2357,47 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
           <t>13-22</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>13-22</t>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>ON</t>
         </is>
       </c>
     </row>
@@ -1569,29 +2409,29 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0930-1830</t>
+          <t>off</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
           <t>7-16</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
       <c r="G25" t="inlineStr">
         <is>
           <t>off</t>
@@ -1599,12 +2439,47 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>自由調配</t>
         </is>
       </c>
     </row>
@@ -1616,17 +2491,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0930-1830</t>
+          <t>off</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1646,12 +2521,47 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>off</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1663,27 +2573,27 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>7-16</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
           <t>0930-1830</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>7-16</t>
-        </is>
-      </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1693,12 +2603,47 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
           <t>13-22</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>13-22</t>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1710,22 +2655,22 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>off</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1740,12 +2685,47 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
           <t>13-22</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>13-22</t>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>AL</t>
         </is>
       </c>
     </row>
@@ -1757,12 +2737,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1772,7 +2752,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1782,17 +2762,52 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>off</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>CL</t>
         </is>
       </c>
     </row>
@@ -1804,22 +2819,22 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>0930-1830</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0930-1830</t>
+          <t>off</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1829,24 +2844,59 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>off</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>CL</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>15/04/2025</t>
+          <t>17/04/2025</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1856,17 +2906,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0930-1830</t>
+          <t>off</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1876,17 +2926,52 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>off</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>AL</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>13-22</t>
+          <t>自由調配</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added half-off to leave types
</commit_message>
<xml_diff>
--- a/schedule_with_senior_editors.xlsx
+++ b/schedule_with_senior_editors.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P31"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,6 +514,16 @@
           <t>Tiffany</t>
         </is>
       </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Caroline</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>CandyC</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -553,7 +563,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>half off</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -594,6 +604,16 @@
       <c r="P2" t="inlineStr">
         <is>
           <t>CL</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -635,7 +655,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -674,6 +694,16 @@
         </is>
       </c>
       <c r="P3" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
         <is>
           <t>10-19</t>
         </is>
@@ -717,7 +747,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>AL</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -756,6 +786,16 @@
         </is>
       </c>
       <c r="P4" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
         <is>
           <t>10-19</t>
         </is>
@@ -842,6 +882,16 @@
           <t>PH</t>
         </is>
       </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -881,7 +931,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -922,6 +972,16 @@
       <c r="P6" t="inlineStr">
         <is>
           <t>ON</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -963,7 +1023,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -1004,6 +1064,16 @@
       <c r="P7" t="inlineStr">
         <is>
           <t>自由調配</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1088,6 +1158,16 @@
           <t>10-19</t>
         </is>
       </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1170,6 +1250,16 @@
           <t>10-19</t>
         </is>
       </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1252,6 +1342,16 @@
           <t>AL</t>
         </is>
       </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1291,7 +1391,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1332,6 +1432,16 @@
       <c r="P11" t="inlineStr">
         <is>
           <t>CL</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1373,7 +1483,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1412,6 +1522,16 @@
         </is>
       </c>
       <c r="P12" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
         <is>
           <t>10-19</t>
         </is>
@@ -1498,6 +1618,16 @@
           <t>10-19</t>
         </is>
       </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1580,6 +1710,16 @@
           <t>PH</t>
         </is>
       </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1619,7 +1759,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1660,6 +1800,16 @@
       <c r="P15" t="inlineStr">
         <is>
           <t>ON</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1701,7 +1851,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1742,6 +1892,16 @@
       <c r="P16" t="inlineStr">
         <is>
           <t>自由調配</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1826,6 +1986,16 @@
           <t>10-19</t>
         </is>
       </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1908,6 +2078,16 @@
           <t>10-19</t>
         </is>
       </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1990,6 +2170,16 @@
           <t>AL</t>
         </is>
       </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2029,7 +2219,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -2070,6 +2260,16 @@
       <c r="P20" t="inlineStr">
         <is>
           <t>CL</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2111,7 +2311,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -2150,6 +2350,16 @@
         </is>
       </c>
       <c r="P21" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
         <is>
           <t>10-19</t>
         </is>
@@ -2236,6 +2446,16 @@
           <t>10-19</t>
         </is>
       </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2318,6 +2538,16 @@
           <t>PH</t>
         </is>
       </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2357,7 +2587,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -2398,6 +2628,16 @@
       <c r="P24" t="inlineStr">
         <is>
           <t>ON</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2439,7 +2679,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -2480,6 +2720,16 @@
       <c r="P25" t="inlineStr">
         <is>
           <t>自由調配</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2521,7 +2771,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -2560,6 +2810,16 @@
         </is>
       </c>
       <c r="P26" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
         <is>
           <t>10-19</t>
         </is>
@@ -2646,6 +2906,16 @@
           <t>10-19</t>
         </is>
       </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2728,6 +2998,16 @@
           <t>AL</t>
         </is>
       </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2767,7 +3047,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2808,6 +3088,16 @@
       <c r="P29" t="inlineStr">
         <is>
           <t>CL</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -2849,7 +3139,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>13-22</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2888,6 +3178,16 @@
         </is>
       </c>
       <c r="P30" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
         <is>
           <t>10-19</t>
         </is>
@@ -2970,6 +3270,16 @@
         </is>
       </c>
       <c r="P31" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
         <is>
           <t>10-19</t>
         </is>

</xml_diff>